<commit_message>
add edf local results
</commit_message>
<xml_diff>
--- a/workspace/gradient_edf_local_validation/gradient_edf_local_validation_schedulables.xlsx
+++ b/workspace/gradient_edf_local_validation/gradient_edf_local_validation_schedulables.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>EDF-L HOPA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>EDF-L GDPA</t>
         </is>
       </c>
@@ -463,6 +468,9 @@
       <c r="D2" t="n">
         <v>50</v>
       </c>
+      <c r="E2" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -477,6 +485,9 @@
       <c r="D3" t="n">
         <v>50</v>
       </c>
+      <c r="E3" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -491,6 +502,9 @@
       <c r="D4" t="n">
         <v>50</v>
       </c>
+      <c r="E4" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -505,6 +519,9 @@
       <c r="D5" t="n">
         <v>50</v>
       </c>
+      <c r="E5" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -519,6 +536,9 @@
       <c r="D6" t="n">
         <v>50</v>
       </c>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -533,6 +553,9 @@
       <c r="D7" t="n">
         <v>50</v>
       </c>
+      <c r="E7" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -547,6 +570,9 @@
       <c r="D8" t="n">
         <v>50</v>
       </c>
+      <c r="E8" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -561,19 +587,25 @@
       <c r="D9" t="n">
         <v>50</v>
       </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>0.6684210526315789</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="E10" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="11">
@@ -581,13 +613,16 @@
         <v>0.6894736842105263</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -595,13 +630,16 @@
         <v>0.7105263157894737</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E12" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -609,13 +647,16 @@
         <v>0.7315789473684211</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="E13" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="14">
@@ -623,13 +664,16 @@
         <v>0.7526315789473684</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="E14" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="15">
@@ -637,13 +681,16 @@
         <v>0.7736842105263158</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E15" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="16">
@@ -651,13 +698,16 @@
         <v>0.7947368421052632</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="E16" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="17">
@@ -665,13 +715,16 @@
         <v>0.8157894736842105</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="E17" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="18">
@@ -679,13 +732,16 @@
         <v>0.8368421052631578</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E18" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="19">
@@ -693,13 +749,16 @@
         <v>0.8578947368421053</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="E19" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="20">
@@ -707,13 +766,16 @@
         <v>0.8789473684210527</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="E20" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="21">
@@ -721,13 +783,16 @@
         <v>0.9</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>